<commit_message>
merged known nest information to tagging data
</commit_message>
<xml_diff>
--- a/data/breeding_data/Tagus/Tagged_KP_breeding.xlsx
+++ b/data/breeding_data/Tagus/Tagged_KP_breeding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afons\Documents\07_PROJECTOS\KP_connectivity_GLS&amp;GPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luketheduke2/Documents/Academic/projects/plover_breeding_movements/data/breeding_data/Tagus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1127EC6A-08B8-423D-BEF9-3F9429438347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516A7CB1-6841-AB49-A1F0-0FEE659AA7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A372F1A3-B55D-404C-BB7F-0E46F89B99D5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{A372F1A3-B55D-404C-BB7F-0E46F89B99D5}"/>
   </bookViews>
   <sheets>
     <sheet name="REF birds" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="65">
   <si>
     <t>D59946</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>D35644</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +282,20 @@
       <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -333,37 +350,27 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FFED7D31"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -377,7 +384,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -665,7 +672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -679,154 +686,154 @@
       <selection activeCell="A2" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="7.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="12"/>
+    <col min="4" max="4" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="16">
+      <c r="D1" s="14">
         <v>2021</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1" s="14">
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>59</v>
       </c>
     </row>
@@ -840,31 +847,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5549A1F8-DE0A-4EE4-9BC2-083B60A2C513}">
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="6"/>
-    <col min="5" max="5" width="10.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="6"/>
+    <col min="5" max="5" width="10.5" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="6"/>
+    <col min="16" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -925,7 +932,7 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -984,7 +991,7 @@
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
@@ -1043,46 +1050,46 @@
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="16">
         <v>38.743648</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="16">
         <v>-8.9755470000000006</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="16">
         <v>2021</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="17">
         <v>44337</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="17">
         <v>44338</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="17">
         <v>44365</v>
       </c>
-      <c r="L4" s="19"/>
-      <c r="M4" s="18" t="s">
+      <c r="L4" s="17"/>
+      <c r="M4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18" t="s">
+      <c r="N4" s="16"/>
+      <c r="O4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="P4" s="3"/>
@@ -1099,7 +1106,7 @@
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
@@ -1158,7 +1165,7 @@
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -1215,7 +1222,7 @@
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1270,7 +1277,7 @@
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -1327,7 +1334,7 @@
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
     </row>
-    <row r="9" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -1384,7 +1391,7 @@
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
     </row>
-    <row r="10" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -1441,7 +1448,7 @@
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
     </row>
-    <row r="11" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -1500,7 +1507,7 @@
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
     </row>
-    <row r="12" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1536,15 +1543,15 @@
       <c r="M12" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="N12" s="14" t="s">
+      <c r="N12" s="12" t="s">
         <v>4</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="3"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
@@ -1554,7 +1561,7 @@
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
     </row>
-    <row r="13" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1594,14 +1601,14 @@
         <v>40</v>
       </c>
       <c r="N13" s="9"/>
-      <c r="O13" s="14" t="s">
+      <c r="O13" s="12" t="s">
         <v>7</v>
       </c>
       <c r="P13" s="3"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="14"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="12"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -1611,39 +1618,43 @@
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18">
+        <v>38.739477999999998</v>
+      </c>
+      <c r="F14" s="18">
+        <v>-8.9921170000000004</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="F15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
       <c r="N15"/>
-      <c r="O15" s="12"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="H16" s="3"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -1651,7 +1662,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H17" s="3"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -1659,7 +1670,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H18" s="3"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -1667,7 +1678,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H19" s="3"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -1675,7 +1686,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H20" s="3"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -1683,19 +1694,19 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H21" s="3"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="22" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H22" s="3"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H23" s="3"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>

</xml_diff>

<commit_message>
started to analyse step-length by breeding status
</commit_message>
<xml_diff>
--- a/data/breeding_data/Tagus/Tagged_KP_breeding.xlsx
+++ b/data/breeding_data/Tagus/Tagged_KP_breeding.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luketheduke2/Documents/Academic/projects/plover_breeding_movements/data/breeding_data/Tagus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516A7CB1-6841-AB49-A1F0-0FEE659AA7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCA7307-AF9C-4644-B139-ADDCD9CA6147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{A372F1A3-B55D-404C-BB7F-0E46F89B99D5}"/>
   </bookViews>
@@ -384,7 +384,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -672,7 +672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -848,7 +848,7 @@
   <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1138,7 @@
         <v>44376</v>
       </c>
       <c r="K5" s="7">
-        <v>44365</v>
+        <v>44395</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="3" t="s">

</xml_diff>